<commit_message>
updated and made more adaptable, added files
</commit_message>
<xml_diff>
--- a/2019LVDataAnalysis.xlsx
+++ b/2019LVDataAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyshen/PycharmProjects/DataAnalysisProgram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1540228C-E486-F443-85BE-A35B6EBFB88C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B5BF46-1692-A34C-A792-0E0711CA4FF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Team" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="481">
   <si>
     <t>Overall Team Data</t>
   </si>
@@ -1519,6 +1519,9 @@
   <si>
     <t>Tried defense but didn't make an impact, didn't seem to do much else</t>
   </si>
+  <si>
+    <t>Rank</t>
+  </si>
 </sst>
 </file>
 
@@ -1573,10 +1576,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC1F2B47-1115-9E45-B9ED-0B711600A679}" name="Table1" displayName="Table1" ref="A2:G50" totalsRowShown="0">
-  <autoFilter ref="A2:G50" xr:uid="{A6929D6E-9C06-544F-928A-96C1F23B28AB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G50">
-    <sortCondition descending="1" ref="G2:G50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC1F2B47-1115-9E45-B9ED-0B711600A679}" name="Table1" displayName="Table1" ref="B2:H50" totalsRowShown="0">
+  <autoFilter ref="B2:H50" xr:uid="{A6929D6E-9C06-544F-928A-96C1F23B28AB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H50">
+    <sortCondition descending="1" ref="H2:H50"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F2AB5E9E-F601-B64E-A17C-F18140F074B9}" name="Team Num"/>
@@ -1876,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1892,386 +1895,434 @@
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>480</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>987</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>5.333333333333333</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4.5238095238095237</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>11.142857142857141</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>35.38095238095238</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>842</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>3.833333333333333</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3.666666666666667</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>11</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>29.666666666666671</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>812</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
         <v>12</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>1836</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>4.3499999999999996</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3.45</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>5.85</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>24.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>7426</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>3.1333333333333329</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3.9333333333333331</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>20.266666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>1197</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>2.8421052631578951</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1.631578947368421</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>9.1578947368421044</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>19.736842105263161</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>696</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>3.7058823529411771</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.1176470588235294</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>9</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>16.764705882352938</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
         <v>3309</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>2.2222222222222219</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2.0555555555555549</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5.666666666666667</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>16.277777777777779</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
         <v>5025</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>4.6111111111111107</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>1.166666666666667</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2.833333333333333</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>15.555555555555561</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>4501</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>1.8421052631578949</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1.4210526315789469</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>7.2631578947368416</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>15.210526315789471</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <v>5285</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>4.5625</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>1.5625</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1.3125</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>15.125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>1388</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>1.8421052631578949</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.47368421052631582</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>9.7894736842105257</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>14.89473684210526</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
         <v>6824</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>0.29411764705882348</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>3.7058823529411771</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2.4705882352941182</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>14.17647058823529</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>2485</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>4.5555555555555554</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1.1111111111111109</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1.166666666666667</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>13.611111111111111</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <v>3009</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>3.333333333333333</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>6.166666666666667</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
         <v>6024</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
@@ -2279,183 +2330,207 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
         <v>60</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>0.125</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>3</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>2.625</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>11.875</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
         <v>5851</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>2.2777777777777781</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1.1111111111111109</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>2.833333333333333</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>10.72222222222222</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
         <v>6822</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>2.736842105263158</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
       <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>2.2105263157894739</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>10.684210526315789</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
         <v>1572</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>2.6842105263157889</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.84210526315789469</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>2.2105263157894739</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>10.10526315789474</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
         <v>7124</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>6</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
         <v>5429</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
         <v>1.944444444444444</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>1.2777777777777779</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>1.666666666666667</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>9.3888888888888875</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
         <v>7424</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>1.833333333333333</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>5</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>8.8333333333333321</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
         <v>7567</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
       <c r="C26">
         <v>0</v>
       </c>
@@ -2463,22 +2538,25 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
         <v>2.6842105263157889</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>8.6842105263157894</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
         <v>991</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
       <c r="C27">
         <v>0</v>
       </c>
@@ -2489,88 +2567,100 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>8.625</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>8.625</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>8.625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
         <v>988</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>5.8823529411764712E-2</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>1.705882352941176</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>2.8235294117647061</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>8.0588235294117645</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
         <v>7613</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
         <v>2.4</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>0.1333333333333333</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>2.6</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>7.8000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
         <v>7425</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>2.3529411764705879</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
       <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>2.8235294117647061</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>7.5294117647058822</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
         <v>585</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -2578,22 +2668,25 @@
         <v>0</v>
       </c>
       <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>1.5263157894736841</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>2.5263157894736841</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>7.1052631578947372</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
         <v>6957</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
       <c r="C32">
         <v>0</v>
       </c>
@@ -2601,137 +2694,155 @@
         <v>0</v>
       </c>
       <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>1.19047619047619</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>3.4285714285714279</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
         <v>3965</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>1.7647058823529409</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
       <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>3</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>6.5294117647058822</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
         <v>6825</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
         <v>0.31578947368421051</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>0.89473684210526316</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>2.6842105263157889</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>1266</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
         <v>1.142857142857143</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>0.14285714285714279</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>2.5714285714285721</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>5.2857142857142856</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
         <v>5474</v>
       </c>
-      <c r="B36">
-        <v>0</v>
-      </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
         <v>1.2</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>1.8</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>5.2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
         <v>6821</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0.5625</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0.5625</v>
       </c>
       <c r="F37">
+        <v>0.5625</v>
+      </c>
+      <c r="G37">
         <v>2.25</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>5.0625</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
         <v>7077</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
       <c r="C38">
         <v>0</v>
       </c>
@@ -2739,160 +2850,181 @@
         <v>0</v>
       </c>
       <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
         <v>0.375</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>3.9375</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>5.0625</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
         <v>7442</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
         <v>3</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
         <v>4322</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
         <v>1.0952380952380949</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
       <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>2.714285714285714</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>4.9047619047619051</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
         <v>3491</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
         <v>1.428571428571429</v>
       </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
       <c r="F41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
         <v>4.8571428571428577</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
         <v>7422</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
         <v>0.61111111111111116</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>0.22222222222222221</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>2.333333333333333</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>4.2222222222222223</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
         <v>7566</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>0.9</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>0.1</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>2.1</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>4.2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
         <v>2647</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>1.75</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>3.666666666666667</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
         <v>7183</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
       <c r="C45">
         <v>0</v>
       </c>
@@ -2900,22 +3032,25 @@
         <v>0</v>
       </c>
       <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>3.2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
         <v>6021</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
       <c r="C46">
         <v>0</v>
       </c>
@@ -2926,42 +3061,48 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
         <v>5049</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
         <v>0.8</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>0.1</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>1.05</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>2.95</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
         <v>7654</v>
       </c>
-      <c r="B48">
-        <v>0</v>
-      </c>
       <c r="C48">
         <v>0</v>
       </c>
@@ -2972,19 +3113,22 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>2.3684210526315792</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>2.3684210526315792</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>2.3684210526315792</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
         <v>6519</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
       <c r="C49">
         <v>0</v>
       </c>
@@ -2995,19 +3139,22 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
         <v>1661</v>
       </c>
-      <c r="B50">
-        <v>0</v>
-      </c>
       <c r="C50">
         <v>0</v>
       </c>
@@ -3018,9 +3165,12 @@
         <v>0</v>
       </c>
       <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
         <v>1.833333333333333</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>1.833333333333333</v>
       </c>
     </row>
@@ -49703,7 +49853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>